<commit_message>
Fix 2026 dates :(
</commit_message>
<xml_diff>
--- a/web/public/data/2026/festes_catalunya_2026.xlsx
+++ b/web/public/data/2026/festes_catalunya_2026.xlsx
@@ -441,7 +441,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2025-01-01</t>
+          <t>2026-01-01</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -458,7 +458,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2025-01-06</t>
+          <t>2026-01-06</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -475,7 +475,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2025-04-03</t>
+          <t>2026-04-03</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -492,7 +492,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2025-04-06</t>
+          <t>2026-04-06</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -509,7 +509,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2025-05-01</t>
+          <t>2026-05-01</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -526,7 +526,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2025-06-24</t>
+          <t>2026-06-24</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -543,7 +543,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2025-08-15</t>
+          <t>2026-08-15</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -560,7 +560,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2025-09-11</t>
+          <t>2026-09-11</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -577,7 +577,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2025-10-12</t>
+          <t>2026-10-12</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -594,7 +594,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2025-12-08</t>
+          <t>2026-12-08</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -611,7 +611,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2025-12-25</t>
+          <t>2026-12-25</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -628,7 +628,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2025-12-26</t>
+          <t>2026-12-26</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">

</xml_diff>